<commit_message>
Can now specify what sprite to show for dialogue.
Author: James Iwamasa.

Srpite can be specified in 4th column of excel sheet. Simply put in
the name of the sprite (no extension like .png), and put the sprite
file into Resources/sprites.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/gameflow.xlsx
+++ b/Typocrypha/Assets/gameflow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rockpolotics\UnityTests\TypocryphaTests\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rockpolotics\unity_projects\GDA\typocrypha\Typocrypha\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>INTRO</t>
   </si>
@@ -38,21 +38,12 @@
     <t>CUTSCENE</t>
   </si>
   <si>
-    <t>This is the last line; goodbye!</t>
-  </si>
-  <si>
     <t>BATTLE</t>
   </si>
   <si>
     <t>NPC</t>
   </si>
   <si>
-    <t>Iris</t>
-  </si>
-  <si>
-    <t>Dahlia</t>
-  </si>
-  <si>
     <t>DIALOGUE</t>
   </si>
   <si>
@@ -71,10 +62,25 @@
     <t>END_GAME</t>
   </si>
   <si>
-    <t>Hi! I'm Dahlia!</t>
-  </si>
-  <si>
-    <t>Don't forget about Iris!</t>
+    <t>Tanuki</t>
+  </si>
+  <si>
+    <t>Frog</t>
+  </si>
+  <si>
+    <t>It'sa me! Tanuki man!</t>
+  </si>
+  <si>
+    <t>tanuki_mario</t>
+  </si>
+  <si>
+    <t>frog_mario</t>
+  </si>
+  <si>
+    <t>Ribbit Ribbit Ribbit Ribbit. Ribbit Ribbit. Riiiiibbbbiiiiiiiiit.</t>
+  </si>
+  <si>
+    <t>Well, goodbye.</t>
   </si>
 </sst>
 </file>
@@ -426,20 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -447,12 +453,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -460,100 +466,109 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feedback for battles (mostly debugging stuff).
Author: James Iwamasa.

Player health is displayed as text.
Player attacks are represented in top left with cast text:
  -if successful, spell text will be displayed.
  -if failed, "Botch" will be displayed.
Enemy health is represented by opacity (as a temporary measure).
Enemy attacks are shown by the enemy getting slightly larger.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/gameflow.xlsx
+++ b/Typocrypha/Assets/gameflow.xlsx
@@ -74,10 +74,10 @@
     <t>Ribbit Ribbit Ribbit Ribbit. Ribbit Ribbit. Riiiiibbbbiiiiiiiiit.</t>
   </si>
   <si>
-    <t>Well, goodbye.</t>
-  </si>
-  <si>
     <t>Slime</t>
+  </si>
+  <si>
+    <t>Well goodbye.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -539,12 +539,9 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
         <v>10</v>
       </c>
     </row>
@@ -558,9 +555,6 @@
       <c r="C13">
         <v>100</v>
       </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -570,10 +564,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>9999</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added sprite_path and max_stagger to EnemyDatabase, made sprite load dynamically
#thetanookihasturned. Set the database so a field can be entered to specify the location of the sprite (relative to resources/sprites) and added a field for maximum stagger in database and enemy stats. the sprite path field could later be used to represent a folder containing all of the enemies sprites. just change resources.load to resources.loadAll in enemy.setStats (could be useful for implementing animation). Set the tanooki's sprite to be tanooki_mario
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/gameflow.xlsx
+++ b/Typocrypha/Assets/gameflow.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rockpolotics\unity_projects\GDA\typocrypha\Typocrypha\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gameflow" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,21 +428,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -450,12 +450,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -493,7 +493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -507,7 +507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -521,12 +521,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -534,45 +534,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>

</xml_diff>